<commit_message>
1. Refactor test flow 2. Add testcase for create supplier
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/Update product.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/Update product.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation\src\main\resources\excels\check_product_detail_sf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8591C337-E3C1-4902-B4B2-F1220FED618F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420C0B5B-A695-42B5-BF19-8788EF42FB39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$77</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="188">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -264,6 +264,38 @@
   </si>
   <si>
     <t>UP_PRODUCT_ENG_G4_06</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Check UI (Language: VIE) and update product
+3. Check UI (Language: VIE) and configure conversion unit
+4. Check UI (Language: VIE) and configure wholesale product
+Storefront:
+1. Access to product detail page by URL
+2. Check UI (All language)
+3. Check 404 Page is shown</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Check UI (Language: ENG) and update product
+3. Check UI (Language: ENG) and configure conversion unit
+4. Check UI (Language: ENG) and configure wholesale product
+Storefront:
+1. Access to product detail page by URL
+2. Check UI (All language)
+3. Check 404 Page is shown</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - without variation
+2. Inactive product and check product detail on storefront</t>
   </si>
   <si>
     <t>Dashboard:
@@ -276,7 +308,7 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
+    - Description
     - Variation (if any)
     - Listing, Selling price
     - Branch name
@@ -293,7 +325,7 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
+    - Description
     - Check sold out mark ...</t>
   </si>
   <si>
@@ -306,7 +338,7 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
+    - Description
     - Variation (if any)
     - Listing, Selling price
     - Branch name
@@ -315,13 +347,49 @@
   <si>
     <t>Dashboard:
 1. Access to dashboard
-2. Check UI (Language: VIE) and update product
-3. Check UI (Language: VIE) and configure conversion unit
-4. Check UI (Language: VIE) and configure wholesale product
+2. Check UI (Language: ENG) and update product
+3. Check UI (Language: ENG) and configure conversion unit
+4. Check UI (Language: ENG) and configure wholesale product
+Storefront:
+1.Access to product detail page by URL
+2. Check UI (All language)
+3. Check all product information:
+    - Product name
+    - Description
+    - Variation (if any)
+    - Listing, Selling price
+    - Branch name
+    - Buy now, Add to cart...</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Check UI (Language: ENG) and update product
+3. Check UI (Language: ENG) and configure conversion unit
+4. Check UI (Language: ENG) and configure wholesale product
 Storefront:
 1. Access to product detail page by URL
 2. Check UI (All language)
-3. Check 404 Page is shown</t>
+3. Check all product information:
+    - Product name
+    - Description
+    - Check sold out mark ...</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Check UI (Language: ENG) and update product
+3. Check UI (Language: ENG) and configure conversion unit
+4. Check UI (Language: ENG) and configure wholesale product
+Storefront:1. Access to product detail page by URL
+2. Check UI (All language)
+3. Check all product information:
+    - Product name
+    - Description
+    - Variation (if any)
+    - Listing, Selling price
+    - Branch name
+    - Buy now, Add to cart…</t>
   </si>
   <si>
     <t>Dashboard:
@@ -334,7 +402,24 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
+    - Description
+    - Variation (if any)
+    - Listing, Selling price
+    - Branch name
+    - Buy now, Add to cart...</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Check UI (Language: ENG) and update product
+3. Check UI (Language: ENG) and configure conversion unit
+4. Check UI (Language: ENG) and configure wholesale product
+Storefront:
+1. Access to product detail page by URL
+2. Check UI (All language)
+3. Check all product information:
+    - Product name
+    - Description
     - Variation (if any)
     - Listing, Selling price
     - Branch name
@@ -351,25 +436,8 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
+    - Description
     - Sold out mark (if variation stock quantity = 0) ...</t>
-  </si>
-  <si>
-    <t>Dashboard:
-1. Access to dashboard
-2. Check UI (Language: ENG) and update product
-3. Check UI (Language: ENG) and configure conversion unit
-4. Check UI (Language: ENG) and configure wholesale product
-Storefront:
-1.Access to product detail page by URL
-2. Check UI (All language)
-3. Check all product information:
-    - Product name
-    - DesUPiption
-    - Variation (if any)
-    - Listing, Selling price
-    - Branch name
-    - Buy now, Add to cart...</t>
   </si>
   <si>
     <t>Dashboard:
@@ -382,84 +450,399 @@
 2. Check UI (All language)
 3. Check all product information:
     - Product name
-    - DesUPiption
-    - Check sold out mark ...</t>
+    - Description
+    - Sold out mark (if variation stock quantity = 0) ...</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G1_05</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - without variation
+2. Delete product and check product is hidden on storefront</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to Dashboard
+2. Delete product
+Storefront:
+1. Access to product detail by URL
+2. Check 404 page is shown</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G1_06</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G1_07</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - without variation
+2. Edit translation (product information + SEO) and check product detail on storefront</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to Dashboard
+2. Edit translation and check UI (Language:VIE)
+Storefront:
+1. Access to product detail by URL
+2. Check translation</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G1_05</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G1_06</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G1_07</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to Dashboard
+2. Edit translation and check UI (Language:ENG)
+Storefront:
+1. Access to product detail by URL
+2. Check translation</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to Dashboard
+2. Change product status
+Storefront:
+1. Access to product detail by URL
+2. Product status
+- Active: Check all informations show correctly
+- Inactive: Check 404 page is shown</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G2_05</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G2_06</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G2_07</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - without variation
+2. Edit translation (product information + SEO) and check product detail on storefront</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - without variation
+2. Inactive product and check product detail on storefront</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - without variation
+2. Delete product and check product is hidden on storefront</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G2_05</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G2_06</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G2_07</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G3_07</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G3_08</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G3_09</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G3_10</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - Variation
+2. Edit translation (Product Information, Variation, SE0)</t>
   </si>
   <si>
     <t>Dashboard:
 1. Access to dashboard
-2. Check UI (Language: ENG) and update product
-3. Check UI (Language: ENG) and configure conversion unit
-4. Check UI (Language: ENG) and configure wholesale product
-Storefront:1. Access to product detail page by URL
-2. Check UI (All language)
-3. Check all product information:
-    - Product name
-    - DesUPiption
-    - Variation (if any)
-    - Listing, Selling price
-    - Branch name
-    - Buy now, Add to cart…</t>
+2. Edit translation and check UI (Language:VIE)
+Storefront:
+1. Access to product detail page by URL
+2. Check translation</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G3_11</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - Variation
+2. Edit translation for each variation (Product Information)</t>
   </si>
   <si>
     <t>Dashboard:
 1. Access to dashboard
-2. Check UI (Language: ENG) and update product
-3. Check UI (Language: ENG) and configure conversion unit
-4. Check UI (Language: ENG) and configure wholesale product
+2. Edit translation for each variation and check UI (Language:VIE)
 Storefront:
 1. Access to product detail page by URL
-2. Check UI (All language)
-3. Check 404 Page is shown</t>
+2. Check translation</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - Variation
+2. Change product status</t>
   </si>
   <si>
     <t>Dashboard:
 1. Access to dashboard
-2. Check UI (Language: ENG) and update product
-3. Check UI (Language: ENG) and configure conversion unit
-4. Check UI (Language: ENG) and configure wholesale product
+2. Change product status
 Storefront:
 1. Access to product detail page by URL
-2. Check UI (All language)
-3. Check all product information:
-    - Product name
-    - DesUPiption
-    - Variation (if any)
-    - Listing, Selling price
-    - Branch name
-    - Buy now, Add to cart...</t>
+2. Check product status
+- Active: Check all informations show correctly
+- Inactive: Check 404 page is shown</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - Variation
+2. Change variation status</t>
+  </si>
+  <si>
+    <t>1. Product type:  Normal - Variation
+2. Delete product and check product is hidden on storefront</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_07</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_08</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_09</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_10</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_11</t>
   </si>
   <si>
     <t>Dashboard:
 1. Access to dashboard
-2. Check UI (Language: ENG) and update product
-3. Check UI (Language: ENG) and configure conversion unit
-4. Check UI (Language: ENG) and configure wholesale product
+2. Edit translation and check UI (Language:ENG)
 Storefront:
 1. Access to product detail page by URL
-2. Check UI (All language)
-3. Check all product information:
-    - Product name
-    - DesUPiption
-    - Sold out mark (if variation stock quantity = 0) ...</t>
-  </si>
-  <si>
-    <t>Update Normal - without variation and check product detail page on storefront</t>
-  </si>
-  <si>
-    <t>Update IMEI - without variation and check product detail page on storefront</t>
-  </si>
-  <si>
-    <t>Update Normal - Variation and check product detail page on storefront</t>
-  </si>
-  <si>
-    <t>Update IMEI - Variation and check product detail page on storefront</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
+2. Check translation</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to dashboard
+2. Edit translation for each variation and check UI (Language:ENG)
+Storefront:
+1. Access to product detail page by URL
+2. Check translation</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G4_07</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G4_08</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G4_09</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G4_10</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_VIE_G4_11</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_07</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_08</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_09</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_10</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_11</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - Variation
+2. Edit translation (Product Information, Variation, SE0)</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - Variation
+2. Edit translation for each variation (Product Information)</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - Variation
+2. Change product status</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - Variation
+2. Change variation status</t>
+  </si>
+  <si>
+    <t>1. Product type:  IMEI - Variation
+2. Delete product and check product is hidden on storefront</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G1_08</t>
+  </si>
+  <si>
+    <t>Dashboard:
+1. Access to Dashboard
+2. Uncheck platform Web
+Storefront:
+1. Access to product detail by URL
+2. Check 404 page is shown</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G2_08</t>
+  </si>
+  <si>
+    <t>1. Product type: IMEI - without variation
+2. Uncheck web platform and check product does not show on storefront</t>
+  </si>
+  <si>
+    <t>1. Product type: Normal - without variation
+2. Uncheck platform Web and check product does not show on storefront</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G3_12</t>
+  </si>
+  <si>
+    <t>1. Product type:  Normal - Variation
+2. Uncheck Web platform and check product does not show on storefront</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page on storefront with no Web platform</t>
+  </si>
+  <si>
+    <t>1. Product type:  IMEI - Variation
+2. Uncheck Web platform and check product does not show on storefront</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when product is deleted</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail when variation status is changed</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when product status is changed</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page after add translation for variation</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation]Check product detail page after add translation for product</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when all variations out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when some variations out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when all variations in-stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when all variations out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when some variations out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - Variation] Check product detail page when all variations in-stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>UP_PRODUCT_ENG_G4_12</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when all variations in-stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when some variations out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when all variations out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when all variations in-stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when some variations out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when all variations out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation]Check product detail page after add translation for product</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page after add translation for variation</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when product status is changed</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail when variation status is changed</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page when product is deleted</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page on storefront with no Web platform</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when in-stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when in-stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[Normal - Variation] Check product detail page after add translation for product</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page after add translation for product</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when product status is changed</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page when product is deleted</t>
+  </si>
+  <si>
+    <t>[Normal - without variation] Check product detail page with no Web platform</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when in-stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when out of stock and check on 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when in-stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when out of stock and uncheck 'Display if out of stock' checkbox</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page after add translation for product</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when product status is changed</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page when product is deleted</t>
+  </si>
+  <si>
+    <t>[IMEI - without variation] Check product detail page with no Web platform</t>
   </si>
 </sst>
 </file>
@@ -812,11 +1195,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1012"/>
+  <dimension ref="A1:G1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -847,1075 +1228,1530 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>79</v>
+        <v>172</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="171" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="E16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="114" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="E23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B32" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="91.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
+        <v>70</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F47" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" ht="91.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="E54" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" t="s">
+        <v>70</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>70</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" ht="91.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
+        <v>69</v>
+      </c>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="E67" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" t="s">
+        <v>70</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" t="s">
+        <v>70</v>
+      </c>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" t="s">
+        <v>70</v>
+      </c>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E71" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F71" t="s">
+        <v>70</v>
+      </c>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="91.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="E77" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="114" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>83</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" t="s">
-        <v>84</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" ht="182.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="148.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="114" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="193.8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" t="s">
-        <v>84</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="159.6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="125.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -7513,8 +8349,206 @@
       <c r="D1012" s="1"/>
       <c r="E1012" s="1"/>
     </row>
+    <row r="1013" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="1"/>
+      <c r="E1013" s="1"/>
+    </row>
+    <row r="1014" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+      <c r="D1014" s="1"/>
+      <c r="E1014" s="1"/>
+    </row>
+    <row r="1015" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="1"/>
+      <c r="E1015" s="1"/>
+    </row>
+    <row r="1016" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+      <c r="E1016" s="1"/>
+    </row>
+    <row r="1017" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1017" s="1"/>
+      <c r="C1017" s="1"/>
+      <c r="D1017" s="1"/>
+      <c r="E1017" s="1"/>
+    </row>
+    <row r="1018" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1018" s="1"/>
+      <c r="C1018" s="1"/>
+      <c r="D1018" s="1"/>
+      <c r="E1018" s="1"/>
+    </row>
+    <row r="1019" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1019" s="1"/>
+      <c r="C1019" s="1"/>
+      <c r="D1019" s="1"/>
+      <c r="E1019" s="1"/>
+    </row>
+    <row r="1020" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1020" s="1"/>
+      <c r="C1020" s="1"/>
+      <c r="D1020" s="1"/>
+      <c r="E1020" s="1"/>
+    </row>
+    <row r="1021" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="1"/>
+      <c r="E1021" s="1"/>
+    </row>
+    <row r="1022" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="1"/>
+      <c r="E1022" s="1"/>
+    </row>
+    <row r="1023" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="1"/>
+      <c r="E1023" s="1"/>
+    </row>
+    <row r="1024" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="1"/>
+      <c r="E1024" s="1"/>
+    </row>
+    <row r="1025" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="1"/>
+      <c r="E1025" s="1"/>
+    </row>
+    <row r="1026" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+      <c r="E1026" s="1"/>
+    </row>
+    <row r="1027" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1027" s="1"/>
+      <c r="C1027" s="1"/>
+      <c r="D1027" s="1"/>
+      <c r="E1027" s="1"/>
+    </row>
+    <row r="1028" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+      <c r="E1028" s="1"/>
+    </row>
+    <row r="1029" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+      <c r="E1029" s="1"/>
+    </row>
+    <row r="1030" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+      <c r="E1030" s="1"/>
+    </row>
+    <row r="1031" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1"/>
+    </row>
+    <row r="1032" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+      <c r="E1032" s="1"/>
+    </row>
+    <row r="1033" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1033" s="1"/>
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+      <c r="E1033" s="1"/>
+    </row>
+    <row r="1034" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1034" s="1"/>
+      <c r="C1034" s="1"/>
+      <c r="D1034" s="1"/>
+      <c r="E1034" s="1"/>
+    </row>
+    <row r="1035" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1035" s="1"/>
+      <c r="C1035" s="1"/>
+      <c r="D1035" s="1"/>
+      <c r="E1035" s="1"/>
+    </row>
+    <row r="1036" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1036" s="1"/>
+      <c r="C1036" s="1"/>
+      <c r="D1036" s="1"/>
+      <c r="E1036" s="1"/>
+    </row>
+    <row r="1037" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1037" s="1"/>
+      <c r="C1037" s="1"/>
+      <c r="D1037" s="1"/>
+      <c r="E1037" s="1"/>
+    </row>
+    <row r="1038" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1038" s="1"/>
+      <c r="C1038" s="1"/>
+      <c r="D1038" s="1"/>
+      <c r="E1038" s="1"/>
+    </row>
+    <row r="1039" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1039" s="1"/>
+      <c r="C1039" s="1"/>
+      <c r="D1039" s="1"/>
+      <c r="E1039" s="1"/>
+    </row>
+    <row r="1040" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1040" s="1"/>
+      <c r="C1040" s="1"/>
+      <c r="D1040" s="1"/>
+      <c r="E1040" s="1"/>
+    </row>
+    <row r="1041" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1041" s="1"/>
+      <c r="C1041" s="1"/>
+      <c r="D1041" s="1"/>
+      <c r="E1041" s="1"/>
+    </row>
+    <row r="1042" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1042" s="1"/>
+      <c r="C1042" s="1"/>
+      <c r="D1042" s="1"/>
+      <c r="E1042" s="1"/>
+    </row>
+    <row r="1043" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1043" s="1"/>
+      <c r="C1043" s="1"/>
+      <c r="D1043" s="1"/>
+      <c r="E1043" s="1"/>
+    </row>
+    <row r="1044" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1044" s="1"/>
+      <c r="C1044" s="1"/>
+      <c r="D1044" s="1"/>
+      <c r="E1044" s="1"/>
+    </row>
+    <row r="1045" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B1045" s="1"/>
+      <c r="C1045" s="1"/>
+      <c r="D1045" s="1"/>
+      <c r="E1045" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="10" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>